<commit_message>
Tons of Bug Fixes, Improvements
- Several Systems now work properly like PowerupSystem & StoreSystem
- Fixed Representation of DebugPanel values
</commit_message>
<xml_diff>
--- a/Armpra/IngameSpecs.xlsx
+++ b/Armpra/IngameSpecs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\armpra\Armpra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E7840C-9C77-48D9-854B-45AB6A8D9CB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D00A0D-CB3A-4F3A-B204-EF6B0096722B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{69554C38-4E87-4DBF-807B-1ECCC7CCB2FE}"/>
+    <workbookView xWindow="2269" yWindow="3505" windowWidth="26083" windowHeight="13924" xr2:uid="{69554C38-4E87-4DBF-807B-1ECCC7CCB2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -852,32 +852,6 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
@@ -1069,6 +1043,32 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1391,13 +1391,13 @@
       <calculatedColumnFormula>(Table1[[#This Row],[Player Level]]^(0.98 * (1 + N$2/1000)))*0.05</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{825B9FA9-DCCA-4DAD-8C38-7F9740461AA7}" name="Bullet Damage Bonus" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{96AC4CB1-B966-4FF7-8CDC-870692BE175B}" name="Attack Speed Period" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{96AC4CB1-B966-4FF7-8CDC-870692BE175B}" name="Attack Speed Period" dataDxfId="11">
       <calculatedColumnFormula>0.9 - (Table1[[#This Row],[Player Level]]^(0.4*(1+M$2/1000)))*0.1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{6DA5BE81-3EE8-4AD8-AB1C-6A3469121A4D}" name="Fire Points" dataDxfId="11">
+    <tableColumn id="9" xr3:uid="{6DA5BE81-3EE8-4AD8-AB1C-6A3469121A4D}" name="Fire Points" dataDxfId="10">
       <calculatedColumnFormula>1 + (Table1[[#This Row],[Player Level]]^1.2)*0.4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0C2275EE-CE6A-4C3F-9462-F1B66977E6F7}" name="Total DPS" dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{0C2275EE-CE6A-4C3F-9462-F1B66977E6F7}" name="Total DPS" dataDxfId="9">
       <calculatedColumnFormula>Table1[[#This Row],[Bullet Damage Bonus]]*Table1[[#This Row],[Attack Speed Period]]*Table1[[#This Row],[Fire Points]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1406,20 +1406,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{303AB1EB-2632-4C38-B19E-4AF8FE132DFF}" name="Table4" displayName="Table4" ref="A1:E101" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{303AB1EB-2632-4C38-B19E-4AF8FE132DFF}" name="Table4" displayName="Table4" ref="A1:E101" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
   <autoFilter ref="A1:E101" xr:uid="{E68EB2F0-42F9-444D-B525-F5150068A076}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6C11904A-9EC3-44DD-8DBC-88B191E8DE44}" name="Map Level" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{70E94984-BDF8-408E-9601-C854152761B0}" name="Enemy Count" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{6C11904A-9EC3-44DD-8DBC-88B191E8DE44}" name="Map Level" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{70E94984-BDF8-408E-9601-C854152761B0}" name="Enemy Count" dataDxfId="3">
       <calculatedColumnFormula>4 + Table4[[#This Row],[Map Level]]^1.05</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9C192A7A-1EA9-4505-A4B7-3C99BE8C2DA2}" name="Max Health Factor" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{9C192A7A-1EA9-4505-A4B7-3C99BE8C2DA2}" name="Max Health Factor" dataDxfId="2">
       <calculatedColumnFormula>0.99  +( Table4[[#This Row],[Map Level]] / 20) ^1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4512C405-AF41-4444-A074-06D6779F0AA8}" name="Damage Factor" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{4512C405-AF41-4444-A074-06D6779F0AA8}" name="Damage Factor" dataDxfId="1">
       <calculatedColumnFormula>0.9 + Table4[[#This Row],[Map Level]]^1.1 / 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{D608E8BC-64D8-49EA-89EF-8C8A51D92950}" name="Attack Speed Factor" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{D608E8BC-64D8-49EA-89EF-8C8A51D92950}" name="Attack Speed Factor" dataDxfId="0">
       <calculatedColumnFormula>0.96 + Table4[[#This Row],[Map Level]]^1.1 / 25</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>